<commit_message>
Upload corrected test cases
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#CGMXX/CGM_XDENT_SOFTWARE_SRL/CGMXFSE/report-checklist.xlsx
+++ b/GATEWAY/A1#111#CGMXX/CGM_XDENT_SOFTWARE_SRL/CGMXFSE/report-checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cgm01-my.sharepoint.com/personal/michele_bukovitz_cgm_com/Documents/Documentazione/FSE/ACCREDITAMENTO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="197" documentId="8_{45AC9EDC-DA0E-934D-A942-652691440C23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4F26C963-6AA7-D84A-9073-29FC68AF84A0}"/>
+  <xr:revisionPtr revIDLastSave="247" documentId="8_{45AC9EDC-DA0E-934D-A942-652691440C23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B67CE248-FF60-F04C-9659-06FC8923F8D1}"/>
   <bookViews>
     <workbookView xWindow="880" yWindow="500" windowWidth="34960" windowHeight="21100" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
     <sheet name="Sheet1" sheetId="5" state="hidden" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">TestCases!$A$9:$T$79</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">TestCases!$A$9:$T$83</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -104,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="963" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="962" uniqueCount="391">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -1595,6 +1595,50 @@
   </si>
   <si>
     <t>ae4c56d221ccfb35</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RAD_CT1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di una futura pubblicazione con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway
+Il Documento CDA2 Referto Radiologia dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 1" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RAD_CT2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di una futura pubblicazione con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway
+Il Documento CDA2 Referto Radiologia dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 2" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RAD_CT3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di una futura pubblicazione con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway
+Il Documento CDA2 Referto Radiologia dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 3" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RAD_CT4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di una futura pubblicazione con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway
+Il Documento CDA2 Referto Radiologia dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 4" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>2024-04-23T09:14:26Z</t>
+  </si>
+  <si>
+    <t>a0643a4878275228</t>
+  </si>
+  <si>
+    <t>0.1.2.3.4.620c9c332101a5bae955c66ae72268fbcd3972766179522c8deede6a249addb7.dab739dc51^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>Il sistema non contiene tutti i dati opzionali rappresentati in modo strutturato, in particolare la sezione conclusioni</t>
   </si>
 </sst>
 </file>
@@ -4511,14 +4555,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:T696"/>
+  <dimension ref="A1:T700"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B74" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="E10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="H75" sqref="H75"/>
+      <selection pane="bottomRight" activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4771,7 +4814,7 @@
     </row>
     <row r="10" spans="1:20" ht="145" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="20">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="B10" s="21" t="s">
         <v>47</v>
@@ -4780,104 +4823,82 @@
         <v>48</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>49</v>
+        <v>379</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>50</v>
+        <v>380</v>
       </c>
       <c r="F10" s="23">
-        <v>45401</v>
+        <v>45405</v>
       </c>
       <c r="G10" s="24" t="s">
-        <v>320</v>
+        <v>387</v>
       </c>
       <c r="H10" s="24" t="s">
-        <v>321</v>
+        <v>388</v>
       </c>
       <c r="I10" s="24" t="s">
-        <v>51</v>
+        <v>389</v>
       </c>
       <c r="J10" s="25" t="s">
         <v>52</v>
       </c>
       <c r="K10" s="25"/>
-      <c r="L10" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="M10" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="N10" s="25" t="s">
-        <v>53</v>
-      </c>
+      <c r="L10" s="25"/>
+      <c r="M10" s="25"/>
+      <c r="N10" s="25"/>
       <c r="O10" s="25"/>
-      <c r="P10" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q10" s="25" t="s">
-        <v>55</v>
-      </c>
+      <c r="P10" s="25"/>
+      <c r="Q10" s="25"/>
       <c r="R10" s="26"/>
       <c r="S10" s="27"/>
       <c r="T10" s="28" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" ht="145" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" ht="145" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="20">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="B11" s="21" t="s">
         <v>47</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>58</v>
+        <v>381</v>
       </c>
       <c r="E11" s="22" t="s">
-        <v>50</v>
+        <v>382</v>
       </c>
       <c r="F11" s="23">
-        <v>45400</v>
-      </c>
-      <c r="G11" s="24" t="s">
-        <v>276</v>
-      </c>
-      <c r="H11" s="24" t="s">
-        <v>277</v>
-      </c>
-      <c r="I11" s="24" t="s">
-        <v>51</v>
-      </c>
+        <v>45406</v>
+      </c>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
       <c r="J11" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="K11" s="25"/>
-      <c r="L11" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="M11" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="N11" s="25" t="s">
-        <v>53</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="K11" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="L11" s="25"/>
+      <c r="M11" s="25"/>
+      <c r="N11" s="25"/>
       <c r="O11" s="25"/>
-      <c r="P11" s="25" t="s">
-        <v>54</v>
-      </c>
+      <c r="P11" s="25"/>
       <c r="Q11" s="25"/>
       <c r="R11" s="26"/>
       <c r="S11" s="27"/>
       <c r="T11" s="28" t="s">
-        <v>56</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="145" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="20">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="B12" s="21" t="s">
         <v>47</v>
@@ -4886,104 +4907,78 @@
         <v>48</v>
       </c>
       <c r="D12" s="21" t="s">
-        <v>59</v>
+        <v>383</v>
       </c>
       <c r="E12" s="22" t="s">
-        <v>60</v>
+        <v>384</v>
       </c>
       <c r="F12" s="23">
-        <v>45401</v>
-      </c>
-      <c r="G12" s="24" t="s">
-        <v>322</v>
-      </c>
-      <c r="H12" s="24" t="s">
-        <v>323</v>
-      </c>
-      <c r="I12" s="24" t="s">
-        <v>51</v>
-      </c>
+        <v>45407</v>
+      </c>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
       <c r="J12" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="K12" s="25"/>
-      <c r="L12" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="M12" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="N12" s="25" t="s">
-        <v>53</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="K12" s="25" t="s">
+        <v>390</v>
+      </c>
+      <c r="L12" s="25"/>
+      <c r="M12" s="25"/>
+      <c r="N12" s="25"/>
       <c r="O12" s="25"/>
-      <c r="P12" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q12" s="25" t="s">
-        <v>55</v>
-      </c>
+      <c r="P12" s="25"/>
+      <c r="Q12" s="25"/>
       <c r="R12" s="26"/>
       <c r="S12" s="27"/>
       <c r="T12" s="28" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" ht="145" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" ht="145" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="20">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="B13" s="21" t="s">
         <v>47</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>61</v>
+        <v>385</v>
       </c>
       <c r="E13" s="22" t="s">
-        <v>60</v>
+        <v>386</v>
       </c>
       <c r="F13" s="23">
-        <v>45400</v>
-      </c>
-      <c r="G13" s="24" t="s">
-        <v>278</v>
-      </c>
-      <c r="H13" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="I13" s="24" t="s">
-        <v>51</v>
-      </c>
+        <v>45408</v>
+      </c>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24"/>
       <c r="J13" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="K13" s="25"/>
-      <c r="L13" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="M13" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="N13" s="25" t="s">
-        <v>53</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="K13" s="25" t="s">
+        <v>390</v>
+      </c>
+      <c r="L13" s="25"/>
+      <c r="M13" s="25"/>
+      <c r="N13" s="25"/>
       <c r="O13" s="25"/>
-      <c r="P13" s="25" t="s">
-        <v>54</v>
-      </c>
+      <c r="P13" s="25"/>
       <c r="Q13" s="25"/>
       <c r="R13" s="26"/>
       <c r="S13" s="27"/>
       <c r="T13" s="28" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" ht="65" thickBot="1" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" ht="145" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="20">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="B14" s="21" t="s">
         <v>47</v>
@@ -4992,18 +4987,26 @@
         <v>48</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="E14" s="22" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="F14" s="23">
         <v>45401</v>
       </c>
-      <c r="G14" s="24"/>
-      <c r="H14" s="24"/>
-      <c r="I14" s="24"/>
-      <c r="J14" s="25"/>
+      <c r="G14" s="24" t="s">
+        <v>320</v>
+      </c>
+      <c r="H14" s="24" t="s">
+        <v>321</v>
+      </c>
+      <c r="I14" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="J14" s="25" t="s">
+        <v>52</v>
+      </c>
       <c r="K14" s="25"/>
       <c r="L14" s="25" t="s">
         <v>52</v>
@@ -5016,22 +5019,18 @@
       </c>
       <c r="O14" s="25"/>
       <c r="P14" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q14" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="R14" s="26" t="s">
-        <v>52</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="Q14" s="25"/>
+      <c r="R14" s="26"/>
       <c r="S14" s="27"/>
       <c r="T14" s="28" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="65" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" ht="145" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="20">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="B15" s="21" t="s">
         <v>47</v>
@@ -5040,19 +5039,23 @@
         <v>57</v>
       </c>
       <c r="D15" s="21" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="E15" s="22" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="F15" s="23">
-        <v>45391</v>
+        <v>45400</v>
       </c>
       <c r="G15" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="H15" s="24"/>
-      <c r="I15" s="24"/>
+        <v>276</v>
+      </c>
+      <c r="H15" s="24" t="s">
+        <v>277</v>
+      </c>
+      <c r="I15" s="24" t="s">
+        <v>51</v>
+      </c>
       <c r="J15" s="25" t="s">
         <v>52</v>
       </c>
@@ -5068,12 +5071,10 @@
       </c>
       <c r="O15" s="25"/>
       <c r="P15" s="25" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="Q15" s="25"/>
-      <c r="R15" s="26" t="s">
-        <v>52</v>
-      </c>
+      <c r="R15" s="26"/>
       <c r="S15" s="27"/>
       <c r="T15" s="28" t="s">
         <v>56</v>
@@ -5081,7 +5082,7 @@
     </row>
     <row r="16" spans="1:20" ht="145" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="20">
-        <v>75</v>
+        <v>39</v>
       </c>
       <c r="B16" s="21" t="s">
         <v>47</v>
@@ -5090,22 +5091,22 @@
         <v>48</v>
       </c>
       <c r="D16" s="21" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="E16" s="22" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="F16" s="23">
         <v>45401</v>
       </c>
       <c r="G16" s="24" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="H16" s="24" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="I16" s="24" t="s">
-        <v>326</v>
+        <v>51</v>
       </c>
       <c r="J16" s="25" t="s">
         <v>52</v>
@@ -5124,42 +5125,40 @@
       <c r="P16" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="Q16" s="25" t="s">
-        <v>55</v>
-      </c>
+      <c r="Q16" s="25"/>
       <c r="R16" s="26"/>
       <c r="S16" s="27"/>
       <c r="T16" s="28" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="129" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" ht="145" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="20">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="B17" s="21" t="s">
         <v>47</v>
       </c>
       <c r="C17" s="21" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="D17" s="21" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="E17" s="22" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="F17" s="23">
-        <v>45401</v>
+        <v>45400</v>
       </c>
       <c r="G17" s="24" t="s">
-        <v>327</v>
+        <v>278</v>
       </c>
       <c r="H17" s="24" t="s">
-        <v>328</v>
+        <v>62</v>
       </c>
       <c r="I17" s="24" t="s">
-        <v>329</v>
+        <v>51</v>
       </c>
       <c r="J17" s="25" t="s">
         <v>52</v>
@@ -5178,18 +5177,16 @@
       <c r="P17" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="Q17" s="25" t="s">
-        <v>55</v>
-      </c>
+      <c r="Q17" s="25"/>
       <c r="R17" s="26"/>
       <c r="S17" s="27"/>
       <c r="T17" s="28" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="113" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" ht="65" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="20">
-        <v>77</v>
+        <v>47</v>
       </c>
       <c r="B18" s="21" t="s">
         <v>47</v>
@@ -5198,26 +5195,18 @@
         <v>48</v>
       </c>
       <c r="D18" s="21" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="E18" s="22" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="F18" s="23">
         <v>45401</v>
       </c>
-      <c r="G18" s="24" t="s">
-        <v>330</v>
-      </c>
-      <c r="H18" s="24" t="s">
-        <v>331</v>
-      </c>
-      <c r="I18" s="24" t="s">
-        <v>332</v>
-      </c>
-      <c r="J18" s="25" t="s">
-        <v>52</v>
-      </c>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="25"/>
       <c r="K18" s="25"/>
       <c r="L18" s="25" t="s">
         <v>52</v>
@@ -5230,45 +5219,41 @@
       </c>
       <c r="O18" s="25"/>
       <c r="P18" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q18" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="R18" s="26"/>
+        <v>65</v>
+      </c>
+      <c r="Q18" s="25"/>
+      <c r="R18" s="26" t="s">
+        <v>52</v>
+      </c>
       <c r="S18" s="27"/>
       <c r="T18" s="28" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="113" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" ht="65" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="20">
-        <v>78</v>
+        <v>48</v>
       </c>
       <c r="B19" s="21" t="s">
         <v>47</v>
       </c>
       <c r="C19" s="21" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="D19" s="21" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="E19" s="22" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="F19" s="23">
-        <v>45401</v>
+        <v>45391</v>
       </c>
       <c r="G19" s="24" t="s">
-        <v>333</v>
-      </c>
-      <c r="H19" s="24" t="s">
-        <v>334</v>
-      </c>
-      <c r="I19" s="24" t="s">
-        <v>335</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
       <c r="J19" s="25" t="s">
         <v>52</v>
       </c>
@@ -5284,20 +5269,20 @@
       </c>
       <c r="O19" s="25"/>
       <c r="P19" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q19" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="R19" s="26"/>
+        <v>65</v>
+      </c>
+      <c r="Q19" s="25"/>
+      <c r="R19" s="26" t="s">
+        <v>52</v>
+      </c>
       <c r="S19" s="27"/>
       <c r="T19" s="28" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="129" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" ht="145" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="20">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B20" s="21" t="s">
         <v>47</v>
@@ -5306,22 +5291,22 @@
         <v>48</v>
       </c>
       <c r="D20" s="21" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="E20" s="22" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="F20" s="23">
         <v>45401</v>
       </c>
       <c r="G20" s="24" t="s">
-        <v>336</v>
+        <v>324</v>
       </c>
       <c r="H20" s="24" t="s">
-        <v>337</v>
+        <v>325</v>
       </c>
       <c r="I20" s="24" t="s">
-        <v>338</v>
+        <v>326</v>
       </c>
       <c r="J20" s="25" t="s">
         <v>52</v>
@@ -5340,9 +5325,7 @@
       <c r="P20" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="Q20" s="25" t="s">
-        <v>55</v>
-      </c>
+      <c r="Q20" s="25"/>
       <c r="R20" s="26"/>
       <c r="S20" s="27"/>
       <c r="T20" s="28" t="s">
@@ -5351,7 +5334,7 @@
     </row>
     <row r="21" spans="1:20" ht="129" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="20">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B21" s="21" t="s">
         <v>47</v>
@@ -5360,22 +5343,22 @@
         <v>48</v>
       </c>
       <c r="D21" s="21" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="E21" s="22" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="F21" s="23">
         <v>45401</v>
       </c>
       <c r="G21" s="24" t="s">
-        <v>339</v>
+        <v>327</v>
       </c>
       <c r="H21" s="24" t="s">
-        <v>340</v>
+        <v>328</v>
       </c>
       <c r="I21" s="24" t="s">
-        <v>341</v>
+        <v>329</v>
       </c>
       <c r="J21" s="25" t="s">
         <v>52</v>
@@ -5394,18 +5377,16 @@
       <c r="P21" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="Q21" s="25" t="s">
-        <v>55</v>
-      </c>
+      <c r="Q21" s="25"/>
       <c r="R21" s="26"/>
       <c r="S21" s="27"/>
       <c r="T21" s="28" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="129" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" ht="113" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="20">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B22" s="21" t="s">
         <v>47</v>
@@ -5414,26 +5395,40 @@
         <v>48</v>
       </c>
       <c r="D22" s="21" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="E22" s="22" t="s">
-        <v>81</v>
-      </c>
-      <c r="F22" s="23"/>
-      <c r="G22" s="24"/>
-      <c r="H22" s="24"/>
-      <c r="I22" s="24"/>
+        <v>73</v>
+      </c>
+      <c r="F22" s="23">
+        <v>45401</v>
+      </c>
+      <c r="G22" s="24" t="s">
+        <v>330</v>
+      </c>
+      <c r="H22" s="24" t="s">
+        <v>331</v>
+      </c>
+      <c r="I22" s="24" t="s">
+        <v>332</v>
+      </c>
       <c r="J22" s="25" t="s">
-        <v>82</v>
-      </c>
-      <c r="K22" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="L22" s="25"/>
-      <c r="M22" s="25"/>
-      <c r="N22" s="25"/>
+        <v>52</v>
+      </c>
+      <c r="K22" s="25"/>
+      <c r="L22" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="M22" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="N22" s="25" t="s">
+        <v>53</v>
+      </c>
       <c r="O22" s="25"/>
-      <c r="P22" s="25"/>
+      <c r="P22" s="25" t="s">
+        <v>54</v>
+      </c>
       <c r="Q22" s="25"/>
       <c r="R22" s="26"/>
       <c r="S22" s="27"/>
@@ -5441,9 +5436,9 @@
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="129" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" ht="113" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="20">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B23" s="21" t="s">
         <v>47</v>
@@ -5452,22 +5447,22 @@
         <v>48</v>
       </c>
       <c r="D23" s="21" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="E23" s="22" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="F23" s="23">
         <v>45401</v>
       </c>
       <c r="G23" s="24" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
       <c r="H23" s="24" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="I23" s="24" t="s">
-        <v>344</v>
+        <v>335</v>
       </c>
       <c r="J23" s="25" t="s">
         <v>52</v>
@@ -5486,18 +5481,16 @@
       <c r="P23" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="Q23" s="25" t="s">
-        <v>55</v>
-      </c>
+      <c r="Q23" s="25"/>
       <c r="R23" s="26"/>
       <c r="S23" s="27"/>
       <c r="T23" s="28" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="113" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" ht="129" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="20">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B24" s="21" t="s">
         <v>47</v>
@@ -5506,26 +5499,40 @@
         <v>48</v>
       </c>
       <c r="D24" s="21" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="E24" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="F24" s="23"/>
-      <c r="G24" s="24"/>
-      <c r="H24" s="24"/>
-      <c r="I24" s="24"/>
+        <v>77</v>
+      </c>
+      <c r="F24" s="23">
+        <v>45401</v>
+      </c>
+      <c r="G24" s="24" t="s">
+        <v>336</v>
+      </c>
+      <c r="H24" s="24" t="s">
+        <v>337</v>
+      </c>
+      <c r="I24" s="24" t="s">
+        <v>338</v>
+      </c>
       <c r="J24" s="25" t="s">
-        <v>82</v>
-      </c>
-      <c r="K24" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="L24" s="25"/>
-      <c r="M24" s="25"/>
-      <c r="N24" s="25"/>
+        <v>52</v>
+      </c>
+      <c r="K24" s="25"/>
+      <c r="L24" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="M24" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="N24" s="25" t="s">
+        <v>53</v>
+      </c>
       <c r="O24" s="25"/>
-      <c r="P24" s="25"/>
+      <c r="P24" s="25" t="s">
+        <v>54</v>
+      </c>
       <c r="Q24" s="25"/>
       <c r="R24" s="26"/>
       <c r="S24" s="27"/>
@@ -5533,9 +5540,9 @@
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="113" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" ht="129" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B25" s="21" t="s">
         <v>47</v>
@@ -5544,22 +5551,22 @@
         <v>48</v>
       </c>
       <c r="D25" s="21" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="E25" s="22" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="F25" s="23">
         <v>45401</v>
       </c>
       <c r="G25" s="24" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="H25" s="24" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="I25" s="24" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="J25" s="25" t="s">
         <v>52</v>
@@ -5578,9 +5585,7 @@
       <c r="P25" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="Q25" s="25" t="s">
-        <v>55</v>
-      </c>
+      <c r="Q25" s="25"/>
       <c r="R25" s="26"/>
       <c r="S25" s="27"/>
       <c r="T25" s="28" t="s">
@@ -5589,7 +5594,7 @@
     </row>
     <row r="26" spans="1:20" ht="129" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="20">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B26" s="21" t="s">
         <v>47</v>
@@ -5598,43 +5603,27 @@
         <v>48</v>
       </c>
       <c r="D26" s="21" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="E26" s="22" t="s">
-        <v>92</v>
-      </c>
-      <c r="F26" s="23">
-        <v>45401</v>
-      </c>
-      <c r="G26" s="24" t="s">
-        <v>348</v>
-      </c>
-      <c r="H26" s="24" t="s">
-        <v>349</v>
-      </c>
-      <c r="I26" s="24" t="s">
-        <v>350</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="F26" s="23"/>
+      <c r="G26" s="24"/>
+      <c r="H26" s="24"/>
+      <c r="I26" s="24"/>
       <c r="J26" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="K26" s="25"/>
-      <c r="L26" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="M26" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="N26" s="25" t="s">
-        <v>53</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="K26" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="L26" s="25"/>
+      <c r="M26" s="25"/>
+      <c r="N26" s="25"/>
       <c r="O26" s="25"/>
-      <c r="P26" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q26" s="25" t="s">
-        <v>55</v>
-      </c>
+      <c r="P26" s="25"/>
+      <c r="Q26" s="25"/>
       <c r="R26" s="26"/>
       <c r="S26" s="27"/>
       <c r="T26" s="28" t="s">
@@ -5643,7 +5632,7 @@
     </row>
     <row r="27" spans="1:20" ht="129" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="20">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B27" s="21" t="s">
         <v>47</v>
@@ -5652,26 +5641,40 @@
         <v>48</v>
       </c>
       <c r="D27" s="21" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="E27" s="22" t="s">
-        <v>94</v>
-      </c>
-      <c r="F27" s="23"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="24"/>
+        <v>85</v>
+      </c>
+      <c r="F27" s="23">
+        <v>45401</v>
+      </c>
+      <c r="G27" s="24" t="s">
+        <v>342</v>
+      </c>
+      <c r="H27" s="24" t="s">
+        <v>343</v>
+      </c>
+      <c r="I27" s="24" t="s">
+        <v>344</v>
+      </c>
       <c r="J27" s="25" t="s">
-        <v>82</v>
-      </c>
-      <c r="K27" s="25" t="s">
-        <v>95</v>
-      </c>
-      <c r="L27" s="25"/>
-      <c r="M27" s="25"/>
-      <c r="N27" s="25"/>
+        <v>52</v>
+      </c>
+      <c r="K27" s="25"/>
+      <c r="L27" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="M27" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="N27" s="25" t="s">
+        <v>53</v>
+      </c>
       <c r="O27" s="25"/>
-      <c r="P27" s="25"/>
+      <c r="P27" s="25" t="s">
+        <v>54</v>
+      </c>
       <c r="Q27" s="25"/>
       <c r="R27" s="26"/>
       <c r="S27" s="27"/>
@@ -5679,9 +5682,9 @@
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="145" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" ht="113" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="20">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B28" s="21" t="s">
         <v>47</v>
@@ -5690,10 +5693,10 @@
         <v>48</v>
       </c>
       <c r="D28" s="21" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="E28" s="22" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="F28" s="23"/>
       <c r="G28" s="24"/>
@@ -5703,7 +5706,7 @@
         <v>82</v>
       </c>
       <c r="K28" s="25" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="L28" s="25"/>
       <c r="M28" s="25"/>
@@ -5717,9 +5720,9 @@
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:20" ht="129" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" ht="113" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="20">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B29" s="21" t="s">
         <v>47</v>
@@ -5728,26 +5731,40 @@
         <v>48</v>
       </c>
       <c r="D29" s="21" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="E29" s="22" t="s">
-        <v>99</v>
-      </c>
-      <c r="F29" s="23"/>
-      <c r="G29" s="24"/>
-      <c r="H29" s="24"/>
-      <c r="I29" s="24"/>
+        <v>90</v>
+      </c>
+      <c r="F29" s="23">
+        <v>45401</v>
+      </c>
+      <c r="G29" s="24" t="s">
+        <v>345</v>
+      </c>
+      <c r="H29" s="24" t="s">
+        <v>346</v>
+      </c>
+      <c r="I29" s="24" t="s">
+        <v>347</v>
+      </c>
       <c r="J29" s="25" t="s">
-        <v>82</v>
-      </c>
-      <c r="K29" s="25" t="s">
-        <v>95</v>
-      </c>
-      <c r="L29" s="25"/>
-      <c r="M29" s="25"/>
-      <c r="N29" s="25"/>
+        <v>52</v>
+      </c>
+      <c r="K29" s="25"/>
+      <c r="L29" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="M29" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="N29" s="25" t="s">
+        <v>53</v>
+      </c>
       <c r="O29" s="25"/>
-      <c r="P29" s="25"/>
+      <c r="P29" s="25" t="s">
+        <v>54</v>
+      </c>
       <c r="Q29" s="25"/>
       <c r="R29" s="26"/>
       <c r="S29" s="27"/>
@@ -5755,9 +5772,9 @@
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="113" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" ht="129" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="20">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B30" s="21" t="s">
         <v>47</v>
@@ -5766,26 +5783,40 @@
         <v>48</v>
       </c>
       <c r="D30" s="21" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="E30" s="22" t="s">
-        <v>101</v>
-      </c>
-      <c r="F30" s="23"/>
-      <c r="G30" s="24"/>
-      <c r="H30" s="24"/>
-      <c r="I30" s="24"/>
+        <v>92</v>
+      </c>
+      <c r="F30" s="23">
+        <v>45401</v>
+      </c>
+      <c r="G30" s="24" t="s">
+        <v>348</v>
+      </c>
+      <c r="H30" s="24" t="s">
+        <v>349</v>
+      </c>
+      <c r="I30" s="24" t="s">
+        <v>350</v>
+      </c>
       <c r="J30" s="25" t="s">
-        <v>82</v>
-      </c>
-      <c r="K30" s="25" t="s">
-        <v>95</v>
-      </c>
-      <c r="L30" s="25"/>
-      <c r="M30" s="25"/>
-      <c r="N30" s="25"/>
+        <v>52</v>
+      </c>
+      <c r="K30" s="25"/>
+      <c r="L30" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="M30" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="N30" s="25" t="s">
+        <v>53</v>
+      </c>
       <c r="O30" s="25"/>
-      <c r="P30" s="25"/>
+      <c r="P30" s="25" t="s">
+        <v>54</v>
+      </c>
       <c r="Q30" s="25"/>
       <c r="R30" s="26"/>
       <c r="S30" s="27"/>
@@ -5793,9 +5824,9 @@
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="113" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" ht="129" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="20">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B31" s="21" t="s">
         <v>47</v>
@@ -5804,10 +5835,10 @@
         <v>48</v>
       </c>
       <c r="D31" s="21" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="E31" s="22" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="F31" s="23"/>
       <c r="G31" s="24"/>
@@ -5831,9 +5862,9 @@
         <v>56</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="129" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" ht="145" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="20">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B32" s="21" t="s">
         <v>47</v>
@@ -5842,10 +5873,10 @@
         <v>48</v>
       </c>
       <c r="D32" s="21" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="E32" s="22" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="F32" s="23"/>
       <c r="G32" s="24"/>
@@ -5871,7 +5902,7 @@
     </row>
     <row r="33" spans="1:20" ht="129" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="20">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B33" s="21" t="s">
         <v>47</v>
@@ -5880,10 +5911,10 @@
         <v>48</v>
       </c>
       <c r="D33" s="21" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="E33" s="22" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="F33" s="23"/>
       <c r="G33" s="24"/>
@@ -5907,9 +5938,9 @@
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:20" ht="129" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" ht="113" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="20">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B34" s="21" t="s">
         <v>47</v>
@@ -5918,10 +5949,10 @@
         <v>48</v>
       </c>
       <c r="D34" s="21" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="E34" s="22" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="F34" s="23"/>
       <c r="G34" s="24"/>
@@ -5945,21 +5976,21 @@
         <v>56</v>
       </c>
     </row>
-    <row r="35" spans="1:20" ht="161" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" ht="113" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="20">
-        <v>147</v>
+        <v>90</v>
       </c>
       <c r="B35" s="21" t="s">
         <v>47</v>
       </c>
       <c r="C35" s="21" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="D35" s="21" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="E35" s="22" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="F35" s="23"/>
       <c r="G35" s="24"/>
@@ -5980,24 +6011,24 @@
       <c r="R35" s="26"/>
       <c r="S35" s="27"/>
       <c r="T35" s="28" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="36" spans="1:20" ht="161" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" ht="129" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="20">
-        <v>148</v>
+        <v>91</v>
       </c>
       <c r="B36" s="21" t="s">
         <v>47</v>
       </c>
       <c r="C36" s="21" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="D36" s="21" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="E36" s="22" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="F36" s="23"/>
       <c r="G36" s="24"/>
@@ -6018,24 +6049,24 @@
       <c r="R36" s="26"/>
       <c r="S36" s="27"/>
       <c r="T36" s="28" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="37" spans="1:20" ht="161" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" ht="129" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="20">
-        <v>149</v>
+        <v>92</v>
       </c>
       <c r="B37" s="21" t="s">
         <v>47</v>
       </c>
       <c r="C37" s="21" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="D37" s="21" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="E37" s="22" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="F37" s="23"/>
       <c r="G37" s="24"/>
@@ -6056,24 +6087,24 @@
       <c r="R37" s="26"/>
       <c r="S37" s="27"/>
       <c r="T37" s="28" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="38" spans="1:20" ht="161" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" ht="129" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="20">
-        <v>150</v>
+        <v>93</v>
       </c>
       <c r="B38" s="21" t="s">
         <v>47</v>
       </c>
       <c r="C38" s="21" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="D38" s="21" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="E38" s="22" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="F38" s="23"/>
       <c r="G38" s="24"/>
@@ -6094,12 +6125,12 @@
       <c r="R38" s="26"/>
       <c r="S38" s="27"/>
       <c r="T38" s="28" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="39" spans="1:20" ht="113" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" ht="161" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="20">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B39" s="21" t="s">
         <v>47</v>
@@ -6108,52 +6139,36 @@
         <v>57</v>
       </c>
       <c r="D39" s="21" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="E39" s="22" t="s">
-        <v>120</v>
-      </c>
-      <c r="F39" s="23">
-        <v>45400</v>
-      </c>
-      <c r="G39" s="24" t="s">
-        <v>279</v>
-      </c>
-      <c r="H39" s="24" t="s">
-        <v>280</v>
-      </c>
-      <c r="I39" s="24" t="s">
-        <v>281</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="F39" s="23"/>
+      <c r="G39" s="24"/>
+      <c r="H39" s="24"/>
+      <c r="I39" s="24"/>
       <c r="J39" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="K39" s="25"/>
-      <c r="L39" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="M39" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="N39" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="O39" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="P39" s="25" t="s">
-        <v>54</v>
-      </c>
+      <c r="K39" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="L39" s="25"/>
+      <c r="M39" s="25"/>
+      <c r="N39" s="25"/>
+      <c r="O39" s="25"/>
+      <c r="P39" s="25"/>
       <c r="Q39" s="25"/>
       <c r="R39" s="26"/>
       <c r="S39" s="27"/>
       <c r="T39" s="28" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="40" spans="1:20" ht="129" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" ht="161" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="20">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B40" s="21" t="s">
         <v>47</v>
@@ -6162,48 +6177,36 @@
         <v>57</v>
       </c>
       <c r="D40" s="21" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="E40" s="22" t="s">
-        <v>122</v>
-      </c>
-      <c r="F40" s="23">
-        <v>45400</v>
-      </c>
-      <c r="G40" s="24" t="s">
-        <v>128</v>
-      </c>
-      <c r="H40" s="24" t="s">
-        <v>129</v>
-      </c>
-      <c r="I40" s="24" t="s">
-        <v>130</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="F40" s="23"/>
+      <c r="G40" s="24"/>
+      <c r="H40" s="24"/>
+      <c r="I40" s="24"/>
       <c r="J40" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="K40" s="25"/>
+        <v>82</v>
+      </c>
+      <c r="K40" s="25" t="s">
+        <v>95</v>
+      </c>
       <c r="L40" s="25"/>
       <c r="M40" s="25"/>
-      <c r="N40" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="O40" s="25" t="s">
-        <v>82</v>
-      </c>
-      <c r="P40" s="25" t="s">
-        <v>54</v>
-      </c>
+      <c r="N40" s="25"/>
+      <c r="O40" s="25"/>
+      <c r="P40" s="25"/>
       <c r="Q40" s="25"/>
       <c r="R40" s="26"/>
       <c r="S40" s="27"/>
       <c r="T40" s="28" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="41" spans="1:20" ht="129" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" ht="161" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="20">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B41" s="21" t="s">
         <v>47</v>
@@ -6212,10 +6215,10 @@
         <v>57</v>
       </c>
       <c r="D41" s="21" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="E41" s="22" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="F41" s="23"/>
       <c r="G41" s="24"/>
@@ -6224,8 +6227,8 @@
       <c r="J41" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="K41" s="33" t="s">
-        <v>125</v>
+      <c r="K41" s="25" t="s">
+        <v>95</v>
       </c>
       <c r="L41" s="25"/>
       <c r="M41" s="25"/>
@@ -6236,12 +6239,12 @@
       <c r="R41" s="26"/>
       <c r="S41" s="27"/>
       <c r="T41" s="28" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="42" spans="1:20" ht="129" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" ht="161" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="20">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B42" s="21" t="s">
         <v>47</v>
@@ -6250,50 +6253,36 @@
         <v>57</v>
       </c>
       <c r="D42" s="21" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="E42" s="22" t="s">
-        <v>127</v>
-      </c>
-      <c r="F42" s="23">
-        <v>45400</v>
-      </c>
-      <c r="G42" s="24" t="s">
-        <v>282</v>
-      </c>
-      <c r="H42" s="24" t="s">
-        <v>283</v>
-      </c>
-      <c r="I42" s="24" t="s">
-        <v>284</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="F42" s="23"/>
+      <c r="G42" s="24"/>
+      <c r="H42" s="24"/>
+      <c r="I42" s="24"/>
       <c r="J42" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="K42" s="25"/>
-      <c r="L42" s="25" t="s">
-        <v>52</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="K42" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="L42" s="25"/>
       <c r="M42" s="25"/>
-      <c r="N42" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="O42" s="25" t="s">
-        <v>82</v>
-      </c>
-      <c r="P42" s="25" t="s">
-        <v>54</v>
-      </c>
+      <c r="N42" s="25"/>
+      <c r="O42" s="25"/>
+      <c r="P42" s="25"/>
       <c r="Q42" s="25"/>
       <c r="R42" s="26"/>
       <c r="S42" s="27"/>
       <c r="T42" s="28" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="43" spans="1:20" ht="129" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" ht="113" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="20">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B43" s="21" t="s">
         <v>47</v>
@@ -6302,22 +6291,22 @@
         <v>57</v>
       </c>
       <c r="D43" s="21" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="E43" s="22" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="F43" s="23">
         <v>45400</v>
       </c>
       <c r="G43" s="24" t="s">
-        <v>286</v>
-      </c>
-      <c r="H43" s="23" t="s">
-        <v>287</v>
+        <v>279</v>
+      </c>
+      <c r="H43" s="24" t="s">
+        <v>280</v>
       </c>
       <c r="I43" s="24" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="J43" s="25" t="s">
         <v>52</v>
@@ -6326,7 +6315,9 @@
       <c r="L43" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="M43" s="25"/>
+      <c r="M43" s="25" t="s">
+        <v>52</v>
+      </c>
       <c r="N43" s="25" t="s">
         <v>53</v>
       </c>
@@ -6343,9 +6334,9 @@
         <v>56</v>
       </c>
     </row>
-    <row r="44" spans="1:20" ht="129" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20" ht="129" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="20">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B44" s="21" t="s">
         <v>47</v>
@@ -6354,30 +6345,28 @@
         <v>57</v>
       </c>
       <c r="D44" s="21" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="E44" s="22" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="F44" s="23">
         <v>45400</v>
       </c>
       <c r="G44" s="24" t="s">
-        <v>285</v>
+        <v>128</v>
       </c>
       <c r="H44" s="24" t="s">
-        <v>290</v>
+        <v>129</v>
       </c>
       <c r="I44" s="24" t="s">
-        <v>289</v>
+        <v>130</v>
       </c>
       <c r="J44" s="25" t="s">
         <v>52</v>
       </c>
       <c r="K44" s="25"/>
-      <c r="L44" s="25" t="s">
-        <v>52</v>
-      </c>
+      <c r="L44" s="25"/>
       <c r="M44" s="25"/>
       <c r="N44" s="25" t="s">
         <v>53</v>
@@ -6395,9 +6384,9 @@
         <v>56</v>
       </c>
     </row>
-    <row r="45" spans="1:20" ht="129" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20" ht="129" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="20">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B45" s="21" t="s">
         <v>47</v>
@@ -6406,10 +6395,10 @@
         <v>57</v>
       </c>
       <c r="D45" s="21" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="E45" s="22" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="F45" s="23"/>
       <c r="G45" s="24"/>
@@ -6418,8 +6407,8 @@
       <c r="J45" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="K45" s="25" t="s">
-        <v>137</v>
+      <c r="K45" s="33" t="s">
+        <v>125</v>
       </c>
       <c r="L45" s="25"/>
       <c r="M45" s="25"/>
@@ -6433,9 +6422,9 @@
         <v>56</v>
       </c>
     </row>
-    <row r="46" spans="1:20" ht="129" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" ht="129" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="20">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B46" s="21" t="s">
         <v>47</v>
@@ -6444,22 +6433,22 @@
         <v>57</v>
       </c>
       <c r="D46" s="21" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="E46" s="22" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="F46" s="23">
         <v>45400</v>
       </c>
       <c r="G46" s="24" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
       <c r="H46" s="24" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
       <c r="I46" s="24" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="J46" s="25" t="s">
         <v>52</v>
@@ -6472,7 +6461,9 @@
       <c r="N46" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="O46" s="25"/>
+      <c r="O46" s="25" t="s">
+        <v>82</v>
+      </c>
       <c r="P46" s="25" t="s">
         <v>54</v>
       </c>
@@ -6483,9 +6474,9 @@
         <v>56</v>
       </c>
     </row>
-    <row r="47" spans="1:20" ht="113" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:20" ht="129" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="20">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B47" s="21" t="s">
         <v>47</v>
@@ -6494,22 +6485,22 @@
         <v>57</v>
       </c>
       <c r="D47" s="21" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="E47" s="22" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="F47" s="23">
         <v>45400</v>
       </c>
       <c r="G47" s="24" t="s">
-        <v>294</v>
-      </c>
-      <c r="H47" s="24" t="s">
-        <v>295</v>
+        <v>286</v>
+      </c>
+      <c r="H47" s="23" t="s">
+        <v>287</v>
       </c>
       <c r="I47" s="24" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="J47" s="25" t="s">
         <v>52</v>
@@ -6522,7 +6513,9 @@
       <c r="N47" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="O47" s="25"/>
+      <c r="O47" s="25" t="s">
+        <v>82</v>
+      </c>
       <c r="P47" s="25" t="s">
         <v>54</v>
       </c>
@@ -6533,9 +6526,9 @@
         <v>56</v>
       </c>
     </row>
-    <row r="48" spans="1:20" ht="113" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:20" ht="129" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="20">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B48" s="21" t="s">
         <v>47</v>
@@ -6544,22 +6537,22 @@
         <v>57</v>
       </c>
       <c r="D48" s="21" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="E48" s="22" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="F48" s="23">
         <v>45400</v>
       </c>
       <c r="G48" s="24" t="s">
-        <v>297</v>
+        <v>285</v>
       </c>
       <c r="H48" s="24" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="I48" s="24" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
       <c r="J48" s="25" t="s">
         <v>52</v>
@@ -6572,7 +6565,9 @@
       <c r="N48" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="O48" s="25"/>
+      <c r="O48" s="25" t="s">
+        <v>82</v>
+      </c>
       <c r="P48" s="25" t="s">
         <v>54</v>
       </c>
@@ -6583,9 +6578,9 @@
         <v>56</v>
       </c>
     </row>
-    <row r="49" spans="1:20" ht="129" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:20" ht="129" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="20">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B49" s="21" t="s">
         <v>47</v>
@@ -6594,38 +6589,26 @@
         <v>57</v>
       </c>
       <c r="D49" s="21" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="E49" s="22" t="s">
-        <v>145</v>
-      </c>
-      <c r="F49" s="23">
-        <v>45400</v>
-      </c>
-      <c r="G49" s="24" t="s">
-        <v>300</v>
-      </c>
-      <c r="H49" s="23" t="s">
-        <v>301</v>
-      </c>
-      <c r="I49" s="24" t="s">
-        <v>302</v>
-      </c>
+        <v>136</v>
+      </c>
+      <c r="F49" s="23"/>
+      <c r="G49" s="24"/>
+      <c r="H49" s="24"/>
+      <c r="I49" s="24"/>
       <c r="J49" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="K49" s="25"/>
-      <c r="L49" s="25" t="s">
-        <v>52</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="K49" s="25" t="s">
+        <v>137</v>
+      </c>
+      <c r="L49" s="25"/>
       <c r="M49" s="25"/>
-      <c r="N49" s="25" t="s">
-        <v>53</v>
-      </c>
+      <c r="N49" s="25"/>
       <c r="O49" s="25"/>
-      <c r="P49" s="25" t="s">
-        <v>54</v>
-      </c>
+      <c r="P49" s="25"/>
       <c r="Q49" s="25"/>
       <c r="R49" s="26"/>
       <c r="S49" s="27"/>
@@ -6633,9 +6616,9 @@
         <v>56</v>
       </c>
     </row>
-    <row r="50" spans="1:20" ht="129" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:20" ht="129" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="20">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B50" s="21" t="s">
         <v>47</v>
@@ -6644,26 +6627,38 @@
         <v>57</v>
       </c>
       <c r="D50" s="21" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="E50" s="22" t="s">
-        <v>147</v>
-      </c>
-      <c r="F50" s="23"/>
-      <c r="G50" s="24"/>
-      <c r="H50" s="24"/>
-      <c r="I50" s="24"/>
+        <v>139</v>
+      </c>
+      <c r="F50" s="23">
+        <v>45400</v>
+      </c>
+      <c r="G50" s="24" t="s">
+        <v>291</v>
+      </c>
+      <c r="H50" s="24" t="s">
+        <v>292</v>
+      </c>
+      <c r="I50" s="24" t="s">
+        <v>293</v>
+      </c>
       <c r="J50" s="25" t="s">
-        <v>82</v>
-      </c>
-      <c r="K50" s="25" t="s">
-        <v>148</v>
-      </c>
-      <c r="L50" s="25"/>
+        <v>52</v>
+      </c>
+      <c r="K50" s="25"/>
+      <c r="L50" s="25" t="s">
+        <v>52</v>
+      </c>
       <c r="M50" s="25"/>
-      <c r="N50" s="25"/>
+      <c r="N50" s="25" t="s">
+        <v>53</v>
+      </c>
       <c r="O50" s="25"/>
-      <c r="P50" s="25"/>
+      <c r="P50" s="25" t="s">
+        <v>54</v>
+      </c>
       <c r="Q50" s="25"/>
       <c r="R50" s="26"/>
       <c r="S50" s="27"/>
@@ -6671,9 +6666,9 @@
         <v>56</v>
       </c>
     </row>
-    <row r="51" spans="1:20" ht="129" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:20" ht="113" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="20">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B51" s="21" t="s">
         <v>47</v>
@@ -6682,26 +6677,38 @@
         <v>57</v>
       </c>
       <c r="D51" s="21" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="E51" s="22" t="s">
-        <v>150</v>
-      </c>
-      <c r="F51" s="23"/>
-      <c r="G51" s="24"/>
-      <c r="H51" s="24"/>
-      <c r="I51" s="24"/>
+        <v>141</v>
+      </c>
+      <c r="F51" s="23">
+        <v>45400</v>
+      </c>
+      <c r="G51" s="24" t="s">
+        <v>294</v>
+      </c>
+      <c r="H51" s="24" t="s">
+        <v>295</v>
+      </c>
+      <c r="I51" s="24" t="s">
+        <v>296</v>
+      </c>
       <c r="J51" s="25" t="s">
-        <v>82</v>
-      </c>
-      <c r="K51" s="25" t="s">
-        <v>148</v>
-      </c>
-      <c r="L51" s="25"/>
+        <v>52</v>
+      </c>
+      <c r="K51" s="25"/>
+      <c r="L51" s="25" t="s">
+        <v>52</v>
+      </c>
       <c r="M51" s="25"/>
-      <c r="N51" s="25"/>
+      <c r="N51" s="25" t="s">
+        <v>53</v>
+      </c>
       <c r="O51" s="25"/>
-      <c r="P51" s="25"/>
+      <c r="P51" s="25" t="s">
+        <v>54</v>
+      </c>
       <c r="Q51" s="25"/>
       <c r="R51" s="26"/>
       <c r="S51" s="27"/>
@@ -6709,9 +6716,9 @@
         <v>56</v>
       </c>
     </row>
-    <row r="52" spans="1:20" ht="129" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:20" ht="113" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A52" s="20">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B52" s="21" t="s">
         <v>47</v>
@@ -6720,26 +6727,38 @@
         <v>57</v>
       </c>
       <c r="D52" s="21" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="E52" s="22" t="s">
-        <v>152</v>
-      </c>
-      <c r="F52" s="23"/>
-      <c r="G52" s="24"/>
-      <c r="H52" s="24"/>
-      <c r="I52" s="24"/>
+        <v>143</v>
+      </c>
+      <c r="F52" s="23">
+        <v>45400</v>
+      </c>
+      <c r="G52" s="24" t="s">
+        <v>297</v>
+      </c>
+      <c r="H52" s="24" t="s">
+        <v>298</v>
+      </c>
+      <c r="I52" s="24" t="s">
+        <v>299</v>
+      </c>
       <c r="J52" s="25" t="s">
-        <v>82</v>
-      </c>
-      <c r="K52" s="25" t="s">
-        <v>148</v>
-      </c>
-      <c r="L52" s="25"/>
+        <v>52</v>
+      </c>
+      <c r="K52" s="25"/>
+      <c r="L52" s="25" t="s">
+        <v>52</v>
+      </c>
       <c r="M52" s="25"/>
-      <c r="N52" s="25"/>
+      <c r="N52" s="25" t="s">
+        <v>53</v>
+      </c>
       <c r="O52" s="25"/>
-      <c r="P52" s="25"/>
+      <c r="P52" s="25" t="s">
+        <v>54</v>
+      </c>
       <c r="Q52" s="25"/>
       <c r="R52" s="26"/>
       <c r="S52" s="27"/>
@@ -6747,9 +6766,9 @@
         <v>56</v>
       </c>
     </row>
-    <row r="53" spans="1:20" ht="129" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:20" ht="129" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A53" s="20">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B53" s="21" t="s">
         <v>47</v>
@@ -6758,26 +6777,38 @@
         <v>57</v>
       </c>
       <c r="D53" s="21" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="E53" s="22" t="s">
-        <v>154</v>
-      </c>
-      <c r="F53" s="23"/>
-      <c r="G53" s="24"/>
-      <c r="H53" s="24"/>
-      <c r="I53" s="24"/>
+        <v>145</v>
+      </c>
+      <c r="F53" s="23">
+        <v>45400</v>
+      </c>
+      <c r="G53" s="24" t="s">
+        <v>300</v>
+      </c>
+      <c r="H53" s="23" t="s">
+        <v>301</v>
+      </c>
+      <c r="I53" s="24" t="s">
+        <v>302</v>
+      </c>
       <c r="J53" s="25" t="s">
-        <v>82</v>
-      </c>
-      <c r="K53" s="25" t="s">
-        <v>148</v>
-      </c>
-      <c r="L53" s="25"/>
+        <v>52</v>
+      </c>
+      <c r="K53" s="25"/>
+      <c r="L53" s="25" t="s">
+        <v>52</v>
+      </c>
       <c r="M53" s="25"/>
-      <c r="N53" s="25"/>
+      <c r="N53" s="25" t="s">
+        <v>53</v>
+      </c>
       <c r="O53" s="25"/>
-      <c r="P53" s="25"/>
+      <c r="P53" s="25" t="s">
+        <v>54</v>
+      </c>
       <c r="Q53" s="25"/>
       <c r="R53" s="26"/>
       <c r="S53" s="27"/>
@@ -6785,9 +6816,9 @@
         <v>56</v>
       </c>
     </row>
-    <row r="54" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:20" ht="129" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A54" s="20">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B54" s="21" t="s">
         <v>47</v>
@@ -6796,10 +6827,10 @@
         <v>57</v>
       </c>
       <c r="D54" s="21" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="E54" s="22" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="F54" s="23"/>
       <c r="G54" s="24"/>
@@ -6823,9 +6854,9 @@
         <v>56</v>
       </c>
     </row>
-    <row r="55" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:20" ht="129" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A55" s="20">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B55" s="21" t="s">
         <v>47</v>
@@ -6834,10 +6865,10 @@
         <v>57</v>
       </c>
       <c r="D55" s="21" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="E55" s="22" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="F55" s="23"/>
       <c r="G55" s="24"/>
@@ -6861,9 +6892,9 @@
         <v>56</v>
       </c>
     </row>
-    <row r="56" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:20" ht="129" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A56" s="20">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B56" s="21" t="s">
         <v>47</v>
@@ -6872,10 +6903,10 @@
         <v>57</v>
       </c>
       <c r="D56" s="21" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="E56" s="22" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F56" s="23"/>
       <c r="G56" s="24"/>
@@ -6899,9 +6930,9 @@
         <v>56</v>
       </c>
     </row>
-    <row r="57" spans="1:20" ht="129" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:20" ht="129" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A57" s="20">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B57" s="21" t="s">
         <v>47</v>
@@ -6910,10 +6941,10 @@
         <v>57</v>
       </c>
       <c r="D57" s="21" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="E57" s="22" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="F57" s="23"/>
       <c r="G57" s="24"/>
@@ -6937,67 +6968,59 @@
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:20" ht="204" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A58" s="20">
-        <v>224</v>
+        <v>166</v>
       </c>
       <c r="B58" s="21" t="s">
-        <v>162</v>
+        <v>47</v>
       </c>
       <c r="C58" s="21" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="D58" s="21" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="E58" s="22" t="s">
-        <v>164</v>
-      </c>
-      <c r="F58" s="23">
-        <v>45401</v>
-      </c>
-      <c r="G58" s="24" t="s">
-        <v>351</v>
-      </c>
-      <c r="H58" s="24" t="s">
-        <v>352</v>
-      </c>
-      <c r="I58" s="24" t="s">
-        <v>353</v>
-      </c>
+        <v>156</v>
+      </c>
+      <c r="F58" s="23"/>
+      <c r="G58" s="24"/>
+      <c r="H58" s="24"/>
+      <c r="I58" s="24"/>
       <c r="J58" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="K58" s="25"/>
+        <v>82</v>
+      </c>
+      <c r="K58" s="25" t="s">
+        <v>148</v>
+      </c>
       <c r="L58" s="25"/>
       <c r="M58" s="25"/>
       <c r="N58" s="25"/>
       <c r="O58" s="25"/>
       <c r="P58" s="25"/>
-      <c r="Q58" s="25" t="s">
-        <v>55</v>
-      </c>
+      <c r="Q58" s="25"/>
       <c r="R58" s="26"/>
       <c r="S58" s="27"/>
       <c r="T58" s="28" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="59" spans="1:20" ht="177" thickBot="1" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="59" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A59" s="20">
-        <v>229</v>
+        <v>167</v>
       </c>
       <c r="B59" s="21" t="s">
-        <v>162</v>
+        <v>47</v>
       </c>
       <c r="C59" s="21" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="D59" s="21" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="E59" s="22" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="F59" s="23"/>
       <c r="G59" s="24"/>
@@ -7007,7 +7030,7 @@
         <v>82</v>
       </c>
       <c r="K59" s="25" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
       <c r="L59" s="25"/>
       <c r="M59" s="25"/>
@@ -7021,121 +7044,85 @@
         <v>56</v>
       </c>
     </row>
-    <row r="60" spans="1:20" ht="177" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A60" s="20">
-        <v>230</v>
+        <v>168</v>
       </c>
       <c r="B60" s="21" t="s">
-        <v>162</v>
+        <v>47</v>
       </c>
       <c r="C60" s="21" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="D60" s="21" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="E60" s="22" t="s">
-        <v>169</v>
-      </c>
-      <c r="F60" s="23">
-        <v>45401</v>
-      </c>
-      <c r="G60" s="24" t="s">
-        <v>356</v>
-      </c>
-      <c r="H60" s="24" t="s">
-        <v>357</v>
-      </c>
-      <c r="I60" s="24" t="s">
-        <v>170</v>
-      </c>
+        <v>160</v>
+      </c>
+      <c r="F60" s="23"/>
+      <c r="G60" s="24"/>
+      <c r="H60" s="24"/>
+      <c r="I60" s="24"/>
       <c r="J60" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="K60" s="25"/>
-      <c r="L60" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="M60" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="N60" s="25" t="s">
-        <v>171</v>
-      </c>
-      <c r="O60" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="P60" s="25" t="s">
-        <v>172</v>
-      </c>
-      <c r="Q60" s="25" t="s">
-        <v>55</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="K60" s="25" t="s">
+        <v>148</v>
+      </c>
+      <c r="L60" s="25"/>
+      <c r="M60" s="25"/>
+      <c r="N60" s="25"/>
+      <c r="O60" s="25"/>
+      <c r="P60" s="25"/>
+      <c r="Q60" s="25"/>
       <c r="R60" s="26"/>
       <c r="S60" s="27"/>
       <c r="T60" s="28" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="61" spans="1:20" ht="225" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:20" ht="129" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A61" s="20">
-        <v>231</v>
+        <v>169</v>
       </c>
       <c r="B61" s="21" t="s">
-        <v>162</v>
+        <v>47</v>
       </c>
       <c r="C61" s="21" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="D61" s="21" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="E61" s="22" t="s">
-        <v>174</v>
-      </c>
-      <c r="F61" s="23">
-        <v>45401</v>
-      </c>
-      <c r="G61" s="24" t="s">
-        <v>358</v>
-      </c>
-      <c r="H61" s="24" t="s">
-        <v>359</v>
-      </c>
-      <c r="I61" s="24" t="s">
-        <v>170</v>
-      </c>
+        <v>160</v>
+      </c>
+      <c r="F61" s="23"/>
+      <c r="G61" s="24"/>
+      <c r="H61" s="24"/>
+      <c r="I61" s="24"/>
       <c r="J61" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="K61" s="25"/>
-      <c r="L61" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="M61" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="N61" s="25" t="s">
-        <v>171</v>
-      </c>
-      <c r="O61" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="P61" s="25" t="s">
-        <v>172</v>
-      </c>
-      <c r="Q61" s="25" t="s">
-        <v>55</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="K61" s="25" t="s">
+        <v>148</v>
+      </c>
+      <c r="L61" s="25"/>
+      <c r="M61" s="25"/>
+      <c r="N61" s="25"/>
+      <c r="O61" s="25"/>
+      <c r="P61" s="25"/>
+      <c r="Q61" s="25"/>
       <c r="R61" s="26"/>
       <c r="S61" s="27"/>
       <c r="T61" s="28" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="62" spans="1:20" ht="193" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:20" ht="204" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A62" s="20">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="B62" s="21" t="s">
         <v>162</v>
@@ -7144,54 +7131,42 @@
         <v>48</v>
       </c>
       <c r="D62" s="21" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="E62" s="22" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="F62" s="23">
         <v>45401</v>
       </c>
       <c r="G62" s="24" t="s">
-        <v>360</v>
+        <v>351</v>
       </c>
       <c r="H62" s="24" t="s">
-        <v>361</v>
+        <v>352</v>
       </c>
       <c r="I62" s="24" t="s">
-        <v>170</v>
+        <v>353</v>
       </c>
       <c r="J62" s="25" t="s">
         <v>52</v>
       </c>
       <c r="K62" s="25"/>
-      <c r="L62" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="M62" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="N62" s="25" t="s">
-        <v>171</v>
-      </c>
-      <c r="O62" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="P62" s="25" t="s">
-        <v>177</v>
-      </c>
-      <c r="Q62" s="25" t="s">
-        <v>55</v>
-      </c>
+      <c r="L62" s="25"/>
+      <c r="M62" s="25"/>
+      <c r="N62" s="25"/>
+      <c r="O62" s="25"/>
+      <c r="P62" s="25"/>
+      <c r="Q62" s="25"/>
       <c r="R62" s="26"/>
       <c r="S62" s="27"/>
       <c r="T62" s="28" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="63" spans="1:20" ht="193" thickBot="1" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20" ht="177" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A63" s="20">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B63" s="21" t="s">
         <v>162</v>
@@ -7200,54 +7175,36 @@
         <v>48</v>
       </c>
       <c r="D63" s="21" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
       <c r="E63" s="22" t="s">
-        <v>179</v>
-      </c>
-      <c r="F63" s="23">
-        <v>45401</v>
-      </c>
-      <c r="G63" s="24" t="s">
-        <v>362</v>
-      </c>
-      <c r="H63" s="24" t="s">
-        <v>363</v>
-      </c>
-      <c r="I63" s="24" t="s">
-        <v>364</v>
-      </c>
+        <v>166</v>
+      </c>
+      <c r="F63" s="23"/>
+      <c r="G63" s="24"/>
+      <c r="H63" s="24"/>
+      <c r="I63" s="24"/>
       <c r="J63" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="K63" s="25"/>
-      <c r="L63" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="M63" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="N63" s="25" t="s">
-        <v>180</v>
-      </c>
-      <c r="O63" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="P63" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="Q63" s="25" t="s">
-        <v>55</v>
-      </c>
+      <c r="K63" s="25" t="s">
+        <v>167</v>
+      </c>
+      <c r="L63" s="25"/>
+      <c r="M63" s="25"/>
+      <c r="N63" s="25"/>
+      <c r="O63" s="25"/>
+      <c r="P63" s="25"/>
+      <c r="Q63" s="25"/>
       <c r="R63" s="26"/>
       <c r="S63" s="27"/>
       <c r="T63" s="28" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="64" spans="1:20" ht="193" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:20" ht="177" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A64" s="20">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B64" s="21" t="s">
         <v>162</v>
@@ -7256,54 +7213,52 @@
         <v>48</v>
       </c>
       <c r="D64" s="21" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
       <c r="E64" s="22" t="s">
-        <v>183</v>
+        <v>169</v>
       </c>
       <c r="F64" s="23">
         <v>45401</v>
       </c>
       <c r="G64" s="24" t="s">
-        <v>365</v>
+        <v>356</v>
       </c>
       <c r="H64" s="24" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="I64" s="24" t="s">
-        <v>364</v>
+        <v>170</v>
       </c>
       <c r="J64" s="25" t="s">
         <v>52</v>
       </c>
       <c r="K64" s="25"/>
       <c r="L64" s="25" t="s">
-        <v>82</v>
+        <v>52</v>
       </c>
       <c r="M64" s="25" t="s">
         <v>52</v>
       </c>
       <c r="N64" s="25" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="O64" s="25" t="s">
         <v>52</v>
       </c>
       <c r="P64" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="Q64" s="25" t="s">
-        <v>55</v>
-      </c>
+        <v>172</v>
+      </c>
+      <c r="Q64" s="25"/>
       <c r="R64" s="26"/>
       <c r="S64" s="27"/>
       <c r="T64" s="28" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="65" spans="1:20" ht="193" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:20" ht="225" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A65" s="20">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="B65" s="21" t="s">
         <v>162</v>
@@ -7312,130 +7267,150 @@
         <v>48</v>
       </c>
       <c r="D65" s="21" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="E65" s="22" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="F65" s="23">
         <v>45401</v>
       </c>
       <c r="G65" s="24" t="s">
-        <v>374</v>
+        <v>358</v>
       </c>
       <c r="H65" s="24" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="I65" s="24" t="s">
-        <v>364</v>
+        <v>170</v>
       </c>
       <c r="J65" s="25" t="s">
         <v>52</v>
       </c>
       <c r="K65" s="25"/>
       <c r="L65" s="25" t="s">
-        <v>82</v>
+        <v>52</v>
       </c>
       <c r="M65" s="25" t="s">
         <v>52</v>
       </c>
       <c r="N65" s="25" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="O65" s="25" t="s">
         <v>52</v>
       </c>
       <c r="P65" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="Q65" s="25" t="s">
-        <v>55</v>
-      </c>
+        <v>172</v>
+      </c>
+      <c r="Q65" s="25"/>
       <c r="R65" s="26"/>
       <c r="S65" s="27"/>
       <c r="T65" s="28" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="66" spans="1:20" ht="264" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:20" ht="193" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A66" s="20">
-        <v>288</v>
+        <v>232</v>
       </c>
       <c r="B66" s="21" t="s">
         <v>162</v>
       </c>
       <c r="C66" s="21" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="D66" s="21" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="E66" s="22" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="F66" s="23">
-        <v>45400</v>
+        <v>45401</v>
       </c>
       <c r="G66" s="24" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="H66" s="24" t="s">
-        <v>303</v>
+        <v>361</v>
       </c>
       <c r="I66" s="24" t="s">
-        <v>304</v>
+        <v>170</v>
       </c>
       <c r="J66" s="25" t="s">
         <v>52</v>
       </c>
       <c r="K66" s="25"/>
-      <c r="L66" s="25"/>
-      <c r="M66" s="25"/>
-      <c r="N66" s="25"/>
-      <c r="O66" s="25"/>
-      <c r="P66" s="25"/>
-      <c r="Q66" s="25" t="s">
-        <v>55</v>
-      </c>
+      <c r="L66" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="M66" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="N66" s="25" t="s">
+        <v>171</v>
+      </c>
+      <c r="O66" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="P66" s="25" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q66" s="25"/>
       <c r="R66" s="26"/>
       <c r="S66" s="27"/>
       <c r="T66" s="28" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="67" spans="1:20" ht="177" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="67" spans="1:20" ht="193" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A67" s="20">
-        <v>293</v>
+        <v>233</v>
       </c>
       <c r="B67" s="21" t="s">
         <v>162</v>
       </c>
       <c r="C67" s="21" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="D67" s="21" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="E67" s="22" t="s">
-        <v>189</v>
-      </c>
-      <c r="F67" s="23"/>
+        <v>179</v>
+      </c>
+      <c r="F67" s="23">
+        <v>45401</v>
+      </c>
       <c r="G67" s="24" t="s">
-        <v>367</v>
-      </c>
-      <c r="H67" s="24"/>
-      <c r="I67" s="24"/>
+        <v>362</v>
+      </c>
+      <c r="H67" s="24" t="s">
+        <v>363</v>
+      </c>
+      <c r="I67" s="24" t="s">
+        <v>364</v>
+      </c>
       <c r="J67" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="K67" s="25"/>
+      <c r="L67" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="K67" s="25" t="s">
-        <v>167</v>
-      </c>
-      <c r="L67" s="25"/>
-      <c r="M67" s="25"/>
-      <c r="N67" s="25"/>
-      <c r="O67" s="25"/>
-      <c r="P67" s="25"/>
+      <c r="M67" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="N67" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="O67" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="P67" s="25" t="s">
+        <v>181</v>
+      </c>
       <c r="Q67" s="25"/>
       <c r="R67" s="26"/>
       <c r="S67" s="27"/>
@@ -7443,117 +7418,117 @@
         <v>56</v>
       </c>
     </row>
-    <row r="68" spans="1:20" ht="177" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:20" ht="193" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A68" s="20">
-        <v>294</v>
+        <v>234</v>
       </c>
       <c r="B68" s="21" t="s">
         <v>162</v>
       </c>
       <c r="C68" s="21" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="D68" s="21" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="E68" s="22" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="F68" s="23">
-        <v>45400</v>
+        <v>45401</v>
       </c>
       <c r="G68" s="24" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="H68" s="24" t="s">
-        <v>305</v>
+        <v>363</v>
       </c>
       <c r="I68" s="24" t="s">
-        <v>170</v>
+        <v>364</v>
       </c>
       <c r="J68" s="25" t="s">
         <v>52</v>
       </c>
       <c r="K68" s="25"/>
       <c r="L68" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="M68" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="M68" s="25"/>
       <c r="N68" s="25" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
       <c r="O68" s="25" t="s">
         <v>52</v>
       </c>
       <c r="P68" s="25" t="s">
-        <v>172</v>
-      </c>
-      <c r="Q68" s="25" t="s">
-        <v>55</v>
-      </c>
+        <v>181</v>
+      </c>
+      <c r="Q68" s="25"/>
       <c r="R68" s="26"/>
       <c r="S68" s="27"/>
       <c r="T68" s="28" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="69" spans="1:20" ht="225" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:20" ht="193" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A69" s="20">
-        <v>295</v>
+        <v>235</v>
       </c>
       <c r="B69" s="21" t="s">
         <v>162</v>
       </c>
       <c r="C69" s="21" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="D69" s="21" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="E69" s="22" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="F69" s="23">
-        <v>45400</v>
+        <v>45401</v>
       </c>
       <c r="G69" s="24" t="s">
-        <v>369</v>
+        <v>374</v>
       </c>
       <c r="H69" s="24" t="s">
-        <v>306</v>
+        <v>363</v>
       </c>
       <c r="I69" s="24" t="s">
-        <v>170</v>
+        <v>364</v>
       </c>
       <c r="J69" s="25" t="s">
         <v>52</v>
       </c>
       <c r="K69" s="25"/>
       <c r="L69" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="M69" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="M69" s="25"/>
       <c r="N69" s="25" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
       <c r="O69" s="25" t="s">
         <v>52</v>
       </c>
       <c r="P69" s="25" t="s">
-        <v>194</v>
-      </c>
-      <c r="Q69" s="25" t="s">
-        <v>55</v>
-      </c>
+        <v>181</v>
+      </c>
+      <c r="Q69" s="25"/>
       <c r="R69" s="26"/>
       <c r="S69" s="27"/>
       <c r="T69" s="28" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="70" spans="1:20" ht="193" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:20" ht="264" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A70" s="20">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="B70" s="21" t="s">
         <v>162</v>
@@ -7562,52 +7537,42 @@
         <v>57</v>
       </c>
       <c r="D70" s="21" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="E70" s="22" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="F70" s="23">
         <v>45400</v>
       </c>
       <c r="G70" s="24" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="H70" s="24" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="I70" s="24" t="s">
-        <v>170</v>
+        <v>304</v>
       </c>
       <c r="J70" s="25" t="s">
         <v>52</v>
       </c>
       <c r="K70" s="25"/>
-      <c r="L70" s="25" t="s">
-        <v>52</v>
-      </c>
+      <c r="L70" s="25"/>
       <c r="M70" s="25"/>
-      <c r="N70" s="25" t="s">
-        <v>171</v>
-      </c>
-      <c r="O70" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="P70" s="25" t="s">
-        <v>308</v>
-      </c>
-      <c r="Q70" s="25" t="s">
-        <v>55</v>
-      </c>
+      <c r="N70" s="25"/>
+      <c r="O70" s="25"/>
+      <c r="P70" s="25"/>
+      <c r="Q70" s="25"/>
       <c r="R70" s="26"/>
       <c r="S70" s="27"/>
       <c r="T70" s="28" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="71" spans="1:20" ht="193" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="71" spans="1:20" ht="177" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A71" s="20">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B71" s="21" t="s">
         <v>162</v>
@@ -7616,54 +7581,38 @@
         <v>57</v>
       </c>
       <c r="D71" s="21" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="E71" s="22" t="s">
-        <v>198</v>
-      </c>
-      <c r="F71" s="23">
-        <v>45400</v>
-      </c>
+        <v>189</v>
+      </c>
+      <c r="F71" s="23"/>
       <c r="G71" s="24" t="s">
-        <v>371</v>
-      </c>
-      <c r="H71" s="24" t="s">
-        <v>309</v>
-      </c>
-      <c r="I71" s="24" t="s">
-        <v>310</v>
-      </c>
+        <v>367</v>
+      </c>
+      <c r="H71" s="24"/>
+      <c r="I71" s="24"/>
       <c r="J71" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="K71" s="25"/>
-      <c r="L71" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="M71" s="25" t="s">
-        <v>82</v>
-      </c>
-      <c r="N71" s="25" t="s">
-        <v>180</v>
-      </c>
-      <c r="O71" s="25" t="s">
-        <v>82</v>
-      </c>
-      <c r="P71" s="25" t="s">
-        <v>200</v>
-      </c>
-      <c r="Q71" s="25" t="s">
-        <v>55</v>
-      </c>
+      <c r="K71" s="25" t="s">
+        <v>167</v>
+      </c>
+      <c r="L71" s="25"/>
+      <c r="M71" s="25"/>
+      <c r="N71" s="25"/>
+      <c r="O71" s="25"/>
+      <c r="P71" s="25"/>
+      <c r="Q71" s="25"/>
       <c r="R71" s="26"/>
       <c r="S71" s="27"/>
       <c r="T71" s="28" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="72" spans="1:20" ht="193" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:20" ht="177" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A72" s="20">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="B72" s="21" t="s">
         <v>162</v>
@@ -7672,54 +7621,50 @@
         <v>57</v>
       </c>
       <c r="D72" s="21" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="E72" s="22" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="F72" s="23">
         <v>45400</v>
       </c>
       <c r="G72" s="24" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="H72" s="24" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="I72" s="24" t="s">
-        <v>312</v>
+        <v>170</v>
       </c>
       <c r="J72" s="25" t="s">
         <v>52</v>
       </c>
       <c r="K72" s="25"/>
       <c r="L72" s="25" t="s">
-        <v>82</v>
-      </c>
-      <c r="M72" s="25" t="s">
-        <v>82</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="M72" s="25"/>
       <c r="N72" s="25" t="s">
-        <v>199</v>
+        <v>171</v>
       </c>
       <c r="O72" s="25" t="s">
-        <v>82</v>
+        <v>52</v>
       </c>
       <c r="P72" s="25" t="s">
-        <v>200</v>
-      </c>
-      <c r="Q72" s="25" t="s">
-        <v>55</v>
-      </c>
+        <v>172</v>
+      </c>
+      <c r="Q72" s="25"/>
       <c r="R72" s="26"/>
       <c r="S72" s="27"/>
       <c r="T72" s="28" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="73" spans="1:20" ht="193" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:20" ht="225" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A73" s="20">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="B73" s="21" t="s">
         <v>162</v>
@@ -7728,75 +7673,71 @@
         <v>57</v>
       </c>
       <c r="D73" s="21" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="E73" s="22" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="F73" s="23">
         <v>45400</v>
       </c>
       <c r="G73" s="24" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="H73" s="24" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="I73" s="24" t="s">
-        <v>314</v>
+        <v>170</v>
       </c>
       <c r="J73" s="25" t="s">
         <v>52</v>
       </c>
       <c r="K73" s="25"/>
       <c r="L73" s="25" t="s">
-        <v>82</v>
-      </c>
-      <c r="M73" s="25" t="s">
-        <v>82</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="M73" s="25"/>
       <c r="N73" s="25" t="s">
-        <v>199</v>
+        <v>171</v>
       </c>
       <c r="O73" s="25" t="s">
-        <v>82</v>
+        <v>52</v>
       </c>
       <c r="P73" s="25" t="s">
-        <v>200</v>
-      </c>
-      <c r="Q73" s="25" t="s">
-        <v>55</v>
-      </c>
+        <v>194</v>
+      </c>
+      <c r="Q73" s="25"/>
       <c r="R73" s="26"/>
       <c r="S73" s="27"/>
       <c r="T73" s="28" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="74" spans="1:20" ht="242.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:20" ht="193" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A74" s="20">
-        <v>328</v>
+        <v>296</v>
       </c>
       <c r="B74" s="21" t="s">
         <v>162</v>
       </c>
       <c r="C74" s="21" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="D74" s="21" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="E74" s="22" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="F74" s="23">
-        <v>45401</v>
+        <v>45400</v>
       </c>
       <c r="G74" s="24" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="H74" s="24" t="s">
-        <v>376</v>
+        <v>307</v>
       </c>
       <c r="I74" s="24" t="s">
         <v>170</v>
@@ -7808,82 +7749,80 @@
       <c r="L74" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="M74" s="25" t="s">
-        <v>52</v>
-      </c>
+      <c r="M74" s="25"/>
       <c r="N74" s="25" t="s">
         <v>171</v>
       </c>
-      <c r="O74" s="25"/>
+      <c r="O74" s="25" t="s">
+        <v>52</v>
+      </c>
       <c r="P74" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q74" s="25" t="s">
-        <v>55</v>
-      </c>
+        <v>308</v>
+      </c>
+      <c r="Q74" s="25"/>
       <c r="R74" s="26"/>
       <c r="S74" s="27"/>
       <c r="T74" s="28" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="75" spans="1:20" ht="242.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:20" ht="193" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A75" s="20">
-        <v>329</v>
+        <v>297</v>
       </c>
       <c r="B75" s="21" t="s">
         <v>162</v>
       </c>
       <c r="C75" s="21" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="D75" s="21" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="E75" s="22" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="F75" s="23">
-        <v>45401</v>
+        <v>45400</v>
       </c>
       <c r="G75" s="24" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="H75" s="24" t="s">
-        <v>378</v>
+        <v>309</v>
       </c>
       <c r="I75" s="24" t="s">
-        <v>170</v>
+        <v>310</v>
       </c>
       <c r="J75" s="25" t="s">
         <v>52</v>
       </c>
       <c r="K75" s="25"/>
       <c r="L75" s="25" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="M75" s="25" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="N75" s="25" t="s">
-        <v>171</v>
-      </c>
-      <c r="O75" s="25"/>
+        <v>180</v>
+      </c>
+      <c r="O75" s="25" t="s">
+        <v>82</v>
+      </c>
       <c r="P75" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q75" s="25" t="s">
-        <v>55</v>
-      </c>
+        <v>200</v>
+      </c>
+      <c r="Q75" s="25"/>
       <c r="R75" s="26"/>
       <c r="S75" s="27"/>
       <c r="T75" s="28" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="76" spans="1:20" ht="242.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:20" ht="193" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A76" s="20">
-        <v>344</v>
+        <v>298</v>
       </c>
       <c r="B76" s="21" t="s">
         <v>162</v>
@@ -7892,26 +7831,42 @@
         <v>57</v>
       </c>
       <c r="D76" s="21" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="E76" s="22" t="s">
-        <v>210</v>
-      </c>
-      <c r="F76" s="23"/>
-      <c r="G76" s="24"/>
-      <c r="H76" s="24"/>
-      <c r="I76" s="24"/>
+        <v>202</v>
+      </c>
+      <c r="F76" s="23">
+        <v>45400</v>
+      </c>
+      <c r="G76" s="24" t="s">
+        <v>372</v>
+      </c>
+      <c r="H76" s="24" t="s">
+        <v>311</v>
+      </c>
+      <c r="I76" s="24" t="s">
+        <v>312</v>
+      </c>
       <c r="J76" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="K76" s="25"/>
+      <c r="L76" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="K76" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="L76" s="25"/>
-      <c r="M76" s="25"/>
-      <c r="N76" s="25"/>
-      <c r="O76" s="25"/>
-      <c r="P76" s="25"/>
+      <c r="M76" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="N76" s="25" t="s">
+        <v>199</v>
+      </c>
+      <c r="O76" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="P76" s="25" t="s">
+        <v>200</v>
+      </c>
       <c r="Q76" s="25"/>
       <c r="R76" s="26"/>
       <c r="S76" s="27"/>
@@ -7919,9 +7874,9 @@
         <v>56</v>
       </c>
     </row>
-    <row r="77" spans="1:20" ht="242.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:20" ht="193" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A77" s="20">
-        <v>345</v>
+        <v>299</v>
       </c>
       <c r="B77" s="21" t="s">
         <v>162</v>
@@ -7930,212 +7885,334 @@
         <v>57</v>
       </c>
       <c r="D77" s="21" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="E77" s="22" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="F77" s="23">
         <v>45400</v>
       </c>
       <c r="G77" s="24" t="s">
-        <v>315</v>
+        <v>373</v>
       </c>
       <c r="H77" s="24" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="I77" s="24" t="s">
-        <v>170</v>
+        <v>314</v>
       </c>
       <c r="J77" s="25" t="s">
         <v>52</v>
       </c>
       <c r="K77" s="25"/>
       <c r="L77" s="25" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="M77" s="25" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="N77" s="25" t="s">
-        <v>171</v>
+        <v>199</v>
       </c>
       <c r="O77" s="25" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="P77" s="25" t="s">
-        <v>213</v>
-      </c>
-      <c r="Q77" s="25" t="s">
-        <v>55</v>
-      </c>
+        <v>200</v>
+      </c>
+      <c r="Q77" s="25"/>
       <c r="R77" s="26"/>
       <c r="S77" s="27"/>
       <c r="T77" s="28" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="78" spans="1:20" ht="144" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:20" ht="242.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A78" s="20">
-        <v>370</v>
+        <v>328</v>
       </c>
       <c r="B78" s="21" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="C78" s="21" t="s">
         <v>48</v>
       </c>
       <c r="D78" s="21" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="E78" s="22" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="F78" s="23">
         <v>45401</v>
       </c>
       <c r="G78" s="24" t="s">
-        <v>354</v>
+        <v>375</v>
       </c>
       <c r="H78" s="24" t="s">
-        <v>355</v>
+        <v>376</v>
       </c>
       <c r="I78" s="24" t="s">
-        <v>353</v>
+        <v>170</v>
       </c>
       <c r="J78" s="25" t="s">
         <v>52</v>
       </c>
       <c r="K78" s="25"/>
-      <c r="L78" s="25"/>
-      <c r="M78" s="25"/>
-      <c r="N78" s="25"/>
+      <c r="L78" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="M78" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="N78" s="25" t="s">
+        <v>171</v>
+      </c>
       <c r="O78" s="25"/>
-      <c r="P78" s="25"/>
-      <c r="Q78" s="25" t="s">
-        <v>55</v>
-      </c>
+      <c r="P78" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q78" s="25"/>
       <c r="R78" s="26"/>
       <c r="S78" s="27"/>
       <c r="T78" s="28" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="79" spans="1:20" ht="160" hidden="1" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="79" spans="1:20" ht="242.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A79" s="20">
-        <v>374</v>
+        <v>329</v>
       </c>
       <c r="B79" s="21" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="C79" s="21" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="D79" s="21" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="E79" s="22" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="F79" s="23">
-        <v>45400</v>
+        <v>45401</v>
       </c>
       <c r="G79" s="24" t="s">
-        <v>317</v>
+        <v>377</v>
       </c>
       <c r="H79" s="24" t="s">
-        <v>318</v>
+        <v>378</v>
       </c>
       <c r="I79" s="24" t="s">
-        <v>319</v>
+        <v>170</v>
       </c>
       <c r="J79" s="25" t="s">
         <v>52</v>
       </c>
       <c r="K79" s="25"/>
-      <c r="L79" s="25"/>
-      <c r="M79" s="25"/>
-      <c r="N79" s="25"/>
+      <c r="L79" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="M79" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="N79" s="25" t="s">
+        <v>171</v>
+      </c>
       <c r="O79" s="25"/>
-      <c r="P79" s="25"/>
-      <c r="Q79" s="25" t="s">
-        <v>55</v>
-      </c>
+      <c r="P79" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q79" s="25"/>
       <c r="R79" s="26"/>
       <c r="S79" s="27"/>
       <c r="T79" s="28" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="80" spans="1:20" ht="242.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>344</v>
+      </c>
+      <c r="B80" s="21" t="s">
+        <v>162</v>
+      </c>
+      <c r="C80" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="D80" s="21" t="s">
+        <v>209</v>
+      </c>
+      <c r="E80" s="22" t="s">
+        <v>210</v>
+      </c>
+      <c r="F80" s="23"/>
+      <c r="G80" s="24"/>
+      <c r="H80" s="24"/>
+      <c r="I80" s="24"/>
+      <c r="J80" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="K80" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="L80" s="25"/>
+      <c r="M80" s="25"/>
+      <c r="N80" s="25"/>
+      <c r="O80" s="25"/>
+      <c r="P80" s="25"/>
+      <c r="Q80" s="25"/>
+      <c r="R80" s="26"/>
+      <c r="S80" s="27"/>
+      <c r="T80" s="28" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="81" spans="1:20" ht="242.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>345</v>
+      </c>
+      <c r="B81" s="21" t="s">
+        <v>162</v>
+      </c>
+      <c r="C81" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="D81" s="21" t="s">
+        <v>211</v>
+      </c>
+      <c r="E81" s="22" t="s">
+        <v>212</v>
+      </c>
+      <c r="F81" s="23">
+        <v>45400</v>
+      </c>
+      <c r="G81" s="24" t="s">
+        <v>315</v>
+      </c>
+      <c r="H81" s="24" t="s">
+        <v>316</v>
+      </c>
+      <c r="I81" s="24" t="s">
+        <v>170</v>
+      </c>
+      <c r="J81" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="K81" s="25"/>
+      <c r="L81" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="M81" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="N81" s="25" t="s">
+        <v>171</v>
+      </c>
+      <c r="O81" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="P81" s="25" t="s">
+        <v>213</v>
+      </c>
+      <c r="Q81" s="25"/>
+      <c r="R81" s="26"/>
+      <c r="S81" s="27"/>
+      <c r="T81" s="28" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="82" spans="1:20" ht="145" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>370</v>
+      </c>
+      <c r="B82" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="C82" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="D82" s="21" t="s">
+        <v>214</v>
+      </c>
+      <c r="E82" s="22" t="s">
+        <v>215</v>
+      </c>
+      <c r="F82" s="23">
+        <v>45401</v>
+      </c>
+      <c r="G82" s="24" t="s">
+        <v>354</v>
+      </c>
+      <c r="H82" s="24" t="s">
+        <v>355</v>
+      </c>
+      <c r="I82" s="24" t="s">
+        <v>353</v>
+      </c>
+      <c r="J82" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="K82" s="25"/>
+      <c r="L82" s="25"/>
+      <c r="M82" s="25"/>
+      <c r="N82" s="25"/>
+      <c r="O82" s="25"/>
+      <c r="P82" s="25"/>
+      <c r="Q82" s="25"/>
+      <c r="R82" s="26"/>
+      <c r="S82" s="27"/>
+      <c r="T82" s="28" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="80" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F80" s="12"/>
-      <c r="G80" s="12"/>
-      <c r="H80" s="12"/>
-      <c r="I80" s="12"/>
-      <c r="J80" s="13"/>
-      <c r="K80" s="13"/>
-      <c r="L80" s="13"/>
-      <c r="M80" s="13"/>
-      <c r="N80" s="13"/>
-      <c r="O80" s="13"/>
-      <c r="P80" s="13"/>
-      <c r="Q80" s="13"/>
-      <c r="R80" s="14"/>
-      <c r="S80" s="2"/>
-      <c r="T80" s="15"/>
-    </row>
-    <row r="81" spans="6:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F81" s="12"/>
-      <c r="G81" s="12"/>
-      <c r="H81" s="12"/>
-      <c r="I81" s="12"/>
-      <c r="J81" s="13"/>
-      <c r="K81" s="13"/>
-      <c r="L81" s="13"/>
-      <c r="M81" s="13"/>
-      <c r="N81" s="13"/>
-      <c r="O81" s="13"/>
-      <c r="P81" s="13"/>
-      <c r="Q81" s="13"/>
-      <c r="R81" s="14"/>
-      <c r="S81" s="2"/>
-      <c r="T81" s="15"/>
-    </row>
-    <row r="82" spans="6:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F82" s="12"/>
-      <c r="G82" s="12"/>
-      <c r="H82" s="12"/>
-      <c r="I82" s="12"/>
-      <c r="J82" s="13"/>
-      <c r="K82" s="13"/>
-      <c r="L82" s="13"/>
-      <c r="M82" s="13"/>
-      <c r="N82" s="13"/>
-      <c r="O82" s="13"/>
-      <c r="P82" s="13"/>
-      <c r="Q82" s="13"/>
-      <c r="R82" s="14"/>
-      <c r="S82" s="2"/>
-      <c r="T82" s="15"/>
-    </row>
-    <row r="83" spans="6:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F83" s="12"/>
-      <c r="G83" s="12"/>
-      <c r="H83" s="12"/>
-      <c r="I83" s="12"/>
-      <c r="J83" s="13"/>
-      <c r="K83" s="13"/>
-      <c r="L83" s="13"/>
-      <c r="M83" s="13"/>
-      <c r="N83" s="13"/>
-      <c r="O83" s="13"/>
-      <c r="P83" s="13"/>
-      <c r="Q83" s="13"/>
-      <c r="R83" s="14"/>
-      <c r="S83" s="2"/>
-      <c r="T83" s="15"/>
-    </row>
-    <row r="84" spans="6:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:20" ht="160" x14ac:dyDescent="0.2">
+      <c r="A83" s="20">
+        <v>374</v>
+      </c>
+      <c r="B83" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="C83" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="D83" s="21" t="s">
+        <v>216</v>
+      </c>
+      <c r="E83" s="22" t="s">
+        <v>217</v>
+      </c>
+      <c r="F83" s="23">
+        <v>45400</v>
+      </c>
+      <c r="G83" s="24" t="s">
+        <v>317</v>
+      </c>
+      <c r="H83" s="24" t="s">
+        <v>318</v>
+      </c>
+      <c r="I83" s="24" t="s">
+        <v>319</v>
+      </c>
+      <c r="J83" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="K83" s="25"/>
+      <c r="L83" s="25"/>
+      <c r="M83" s="25"/>
+      <c r="N83" s="25"/>
+      <c r="O83" s="25"/>
+      <c r="P83" s="25"/>
+      <c r="Q83" s="25"/>
+      <c r="R83" s="26"/>
+      <c r="S83" s="27"/>
+      <c r="T83" s="28" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="84" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F84" s="12"/>
       <c r="G84" s="12"/>
       <c r="H84" s="12"/>
@@ -8152,7 +8229,7 @@
       <c r="S84" s="2"/>
       <c r="T84" s="15"/>
     </row>
-    <row r="85" spans="6:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F85" s="12"/>
       <c r="G85" s="12"/>
       <c r="H85" s="12"/>
@@ -8169,7 +8246,7 @@
       <c r="S85" s="2"/>
       <c r="T85" s="15"/>
     </row>
-    <row r="86" spans="6:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F86" s="12"/>
       <c r="G86" s="12"/>
       <c r="H86" s="12"/>
@@ -8186,7 +8263,7 @@
       <c r="S86" s="2"/>
       <c r="T86" s="15"/>
     </row>
-    <row r="87" spans="6:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F87" s="12"/>
       <c r="G87" s="12"/>
       <c r="H87" s="12"/>
@@ -8203,7 +8280,7 @@
       <c r="S87" s="2"/>
       <c r="T87" s="15"/>
     </row>
-    <row r="88" spans="6:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F88" s="12"/>
       <c r="G88" s="12"/>
       <c r="H88" s="12"/>
@@ -8220,7 +8297,7 @@
       <c r="S88" s="2"/>
       <c r="T88" s="15"/>
     </row>
-    <row r="89" spans="6:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F89" s="12"/>
       <c r="G89" s="12"/>
       <c r="H89" s="12"/>
@@ -8237,7 +8314,7 @@
       <c r="S89" s="2"/>
       <c r="T89" s="15"/>
     </row>
-    <row r="90" spans="6:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F90" s="12"/>
       <c r="G90" s="12"/>
       <c r="H90" s="12"/>
@@ -8254,7 +8331,7 @@
       <c r="S90" s="2"/>
       <c r="T90" s="15"/>
     </row>
-    <row r="91" spans="6:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F91" s="12"/>
       <c r="G91" s="12"/>
       <c r="H91" s="12"/>
@@ -8271,7 +8348,7 @@
       <c r="S91" s="2"/>
       <c r="T91" s="15"/>
     </row>
-    <row r="92" spans="6:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F92" s="12"/>
       <c r="G92" s="12"/>
       <c r="H92" s="12"/>
@@ -8288,7 +8365,7 @@
       <c r="S92" s="2"/>
       <c r="T92" s="15"/>
     </row>
-    <row r="93" spans="6:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F93" s="12"/>
       <c r="G93" s="12"/>
       <c r="H93" s="12"/>
@@ -8305,7 +8382,7 @@
       <c r="S93" s="2"/>
       <c r="T93" s="15"/>
     </row>
-    <row r="94" spans="6:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F94" s="12"/>
       <c r="G94" s="12"/>
       <c r="H94" s="12"/>
@@ -8322,7 +8399,7 @@
       <c r="S94" s="2"/>
       <c r="T94" s="15"/>
     </row>
-    <row r="95" spans="6:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F95" s="12"/>
       <c r="G95" s="12"/>
       <c r="H95" s="12"/>
@@ -8339,7 +8416,7 @@
       <c r="S95" s="2"/>
       <c r="T95" s="15"/>
     </row>
-    <row r="96" spans="6:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F96" s="12"/>
       <c r="G96" s="12"/>
       <c r="H96" s="12"/>
@@ -11468,16 +11545,72 @@
       <c r="T279" s="15"/>
     </row>
     <row r="280" spans="6:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="T280" s="13"/>
+      <c r="F280" s="12"/>
+      <c r="G280" s="12"/>
+      <c r="H280" s="12"/>
+      <c r="I280" s="12"/>
+      <c r="J280" s="13"/>
+      <c r="K280" s="13"/>
+      <c r="L280" s="13"/>
+      <c r="M280" s="13"/>
+      <c r="N280" s="13"/>
+      <c r="O280" s="13"/>
+      <c r="P280" s="13"/>
+      <c r="Q280" s="13"/>
+      <c r="R280" s="14"/>
+      <c r="S280" s="2"/>
+      <c r="T280" s="15"/>
     </row>
     <row r="281" spans="6:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="T281" s="13"/>
+      <c r="F281" s="12"/>
+      <c r="G281" s="12"/>
+      <c r="H281" s="12"/>
+      <c r="I281" s="12"/>
+      <c r="J281" s="13"/>
+      <c r="K281" s="13"/>
+      <c r="L281" s="13"/>
+      <c r="M281" s="13"/>
+      <c r="N281" s="13"/>
+      <c r="O281" s="13"/>
+      <c r="P281" s="13"/>
+      <c r="Q281" s="13"/>
+      <c r="R281" s="14"/>
+      <c r="S281" s="2"/>
+      <c r="T281" s="15"/>
     </row>
     <row r="282" spans="6:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="T282" s="13"/>
+      <c r="F282" s="12"/>
+      <c r="G282" s="12"/>
+      <c r="H282" s="12"/>
+      <c r="I282" s="12"/>
+      <c r="J282" s="13"/>
+      <c r="K282" s="13"/>
+      <c r="L282" s="13"/>
+      <c r="M282" s="13"/>
+      <c r="N282" s="13"/>
+      <c r="O282" s="13"/>
+      <c r="P282" s="13"/>
+      <c r="Q282" s="13"/>
+      <c r="R282" s="14"/>
+      <c r="S282" s="2"/>
+      <c r="T282" s="15"/>
     </row>
     <row r="283" spans="6:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="T283" s="13"/>
+      <c r="F283" s="12"/>
+      <c r="G283" s="12"/>
+      <c r="H283" s="12"/>
+      <c r="I283" s="12"/>
+      <c r="J283" s="13"/>
+      <c r="K283" s="13"/>
+      <c r="L283" s="13"/>
+      <c r="M283" s="13"/>
+      <c r="N283" s="13"/>
+      <c r="O283" s="13"/>
+      <c r="P283" s="13"/>
+      <c r="Q283" s="13"/>
+      <c r="R283" s="14"/>
+      <c r="S283" s="2"/>
+      <c r="T283" s="15"/>
     </row>
     <row r="284" spans="6:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="T284" s="13"/>
@@ -12718,14 +12851,20 @@
     <row r="696" spans="20:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="T696" s="13"/>
     </row>
+    <row r="697" spans="20:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T697" s="13"/>
+    </row>
+    <row r="698" spans="20:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T698" s="13"/>
+    </row>
+    <row r="699" spans="20:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T699" s="13"/>
+    </row>
+    <row r="700" spans="20:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T700" s="13"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A9:T79" xr:uid="{00000000-0009-0000-0000-000002000000}">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="RAD"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A9:T83" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <mergeCells count="7">
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A2:B2"/>
@@ -12745,13 +12884,13 @@
           <x14:formula1>
             <xm:f>Sheet1!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>J10 L12 O10 L10 J12 O12 L79:M79 O79 L15:M57 J14:J57 O48:O57 O14:O46 J79</xm:sqref>
+          <xm:sqref>O14 L16 L14 J83 J16 O16 L83:M83 O83 L19:M61 J18:J61 O52:O61 O18:O50 J14</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000001000000}">
           <x14:formula1>
             <xm:f>Sheet1!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>Q10:Q57 Q78:Q79 Q66</xm:sqref>
+          <xm:sqref>Q70 Q82:Q83 Q14:Q61</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>